<commit_message>
update meeting notes Mar 12
</commit_message>
<xml_diff>
--- a/Performance_20250312.xlsx
+++ b/Performance_20250312.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/menghan/Documents/PaperIdeas/Yining/water_transfer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{844AD52A-CA51-014A-A042-B8EA677ED8F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{518EA91C-4934-8744-8F63-E9011FEDF86A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6200" yWindow="-28300" windowWidth="66240" windowHeight="26920" xr2:uid="{D2BCBF52-8D4E-3A4A-B17F-CA6535631DFE}"/>
+    <workbookView xWindow="980" yWindow="1000" windowWidth="34860" windowHeight="21900" xr2:uid="{D2BCBF52-8D4E-3A4A-B17F-CA6535631DFE}"/>
   </bookViews>
   <sheets>
     <sheet name="Eastern" sheetId="1" r:id="rId1"/>
     <sheet name="Central" sheetId="2" r:id="rId2"/>
     <sheet name="All" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -363,18 +363,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -384,6 +380,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1089,8 +1090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4CF9A21-AF86-B74A-8442-062CB03E78B5}">
   <dimension ref="A1:K75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1100,250 +1101,250 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="15" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>0.92927484333034904</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>0.86956521739130399</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>0.70707070707070696</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>0.77994428969359297</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>0.92211280214861202</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>0.83832335329341301</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>0.7</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>0.76294277929155296</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>0.93375111906893404</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>0.85987261146496796</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>0.72192513368983902</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>0.78488372093023195</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>0.91853178155774395</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>0.78609625668449201</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>0.74242424242424199</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>0.763636363636363</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>0.93017009847806598</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>0.84491978609625595</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>0.76328502415458899</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>0.80203045685279095</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>0.93196060877349995</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>0.881987577639751</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <v>0.71356783919597899</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>0.78888888888888897</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <v>0.94717994628469104</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>0.89090909090908998</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <v>0.78191489361702105</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <v>0.83286118980169899</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="5">
         <v>0.92658907788719702</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <v>0.84090909090909005</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="5">
         <v>0.73267326732673199</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="5">
         <v>0.78306878306878303</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <v>0.937332139659803</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <v>0.87830687830687804</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="5">
         <v>0.77934272300469398</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <v>0.82587064676616895</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="6">
         <v>0.93189964157706096</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="6">
         <v>0.83684210526315705</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="6">
         <v>0.77941176470588203</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="6">
         <v>0.807106598984771</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="5">
         <f>AVERAGE(B5:B14)</f>
         <v>0.9308802058765957</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="5">
         <f>AVERAGE(C5:C14)</f>
         <v>0.85277319679583974</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="5">
         <f>AVERAGE(D5:D14)</f>
         <v>0.74216155951896856</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="5">
         <f>AVERAGE(E5:E14)</f>
         <v>0.79312337179148429</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
@@ -2186,34 +2187,34 @@
       <c r="A54">
         <v>24</v>
       </c>
-      <c r="B54" s="9" t="s">
+      <c r="B54" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C54" s="10" t="s">
+      <c r="C54" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D54" s="10" t="s">
+      <c r="D54" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E54" s="10" t="s">
+      <c r="E54" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F54" s="10" t="s">
+      <c r="F54" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="G54" s="10" t="s">
+      <c r="G54" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="H54" s="10" t="s">
+      <c r="H54" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="I54" s="10" t="s">
+      <c r="I54" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="J54" s="10" t="s">
+      <c r="J54" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="K54" s="11" t="s">
+      <c r="K54" s="9" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2221,34 +2222,34 @@
       <c r="A55">
         <v>25</v>
       </c>
-      <c r="B55" s="12" t="s">
+      <c r="B55" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C55" s="8" t="s">
+      <c r="C55" t="s">
         <v>44</v>
       </c>
-      <c r="D55" s="8" t="s">
+      <c r="D55" t="s">
         <v>43</v>
       </c>
-      <c r="E55" s="8" t="s">
+      <c r="E55" t="s">
         <v>42</v>
       </c>
-      <c r="F55" s="8" t="s">
+      <c r="F55" t="s">
         <v>43</v>
       </c>
-      <c r="G55" s="8" t="s">
+      <c r="G55" t="s">
         <v>42</v>
       </c>
-      <c r="H55" s="8" t="s">
+      <c r="H55" t="s">
         <v>42</v>
       </c>
-      <c r="I55" s="8" t="s">
+      <c r="I55" t="s">
         <v>42</v>
       </c>
-      <c r="J55" s="8" t="s">
+      <c r="J55" t="s">
         <v>42</v>
       </c>
-      <c r="K55" s="13" t="s">
+      <c r="K55" s="11" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2256,34 +2257,34 @@
       <c r="A56">
         <v>26</v>
       </c>
-      <c r="B56" s="12" t="s">
+      <c r="B56" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C56" s="8" t="s">
+      <c r="C56" t="s">
         <v>42</v>
       </c>
-      <c r="D56" s="8" t="s">
+      <c r="D56" t="s">
         <v>45</v>
       </c>
-      <c r="E56" s="8" t="s">
+      <c r="E56" t="s">
         <v>44</v>
       </c>
-      <c r="F56" s="8" t="s">
+      <c r="F56" t="s">
         <v>45</v>
       </c>
-      <c r="G56" s="8" t="s">
+      <c r="G56" t="s">
         <v>44</v>
       </c>
-      <c r="H56" s="8" t="s">
+      <c r="H56" t="s">
         <v>44</v>
       </c>
-      <c r="I56" s="8" t="s">
+      <c r="I56" t="s">
         <v>45</v>
       </c>
-      <c r="J56" s="8" t="s">
+      <c r="J56" t="s">
         <v>45</v>
       </c>
-      <c r="K56" s="13" t="s">
+      <c r="K56" s="11" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2291,34 +2292,34 @@
       <c r="A57">
         <v>27</v>
       </c>
-      <c r="B57" s="12" t="s">
+      <c r="B57" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C57" s="8" t="s">
+      <c r="C57" t="s">
         <v>45</v>
       </c>
-      <c r="D57" s="8" t="s">
+      <c r="D57" t="s">
         <v>44</v>
       </c>
-      <c r="E57" s="8" t="s">
+      <c r="E57" t="s">
         <v>45</v>
       </c>
-      <c r="F57" s="8" t="s">
+      <c r="F57" t="s">
         <v>44</v>
       </c>
-      <c r="G57" s="8" t="s">
+      <c r="G57" t="s">
         <v>45</v>
       </c>
-      <c r="H57" s="8" t="s">
+      <c r="H57" t="s">
         <v>45</v>
       </c>
-      <c r="I57" s="8" t="s">
+      <c r="I57" t="s">
         <v>46</v>
       </c>
-      <c r="J57" s="8" t="s">
+      <c r="J57" t="s">
         <v>44</v>
       </c>
-      <c r="K57" s="13" t="s">
+      <c r="K57" s="11" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2326,39 +2327,39 @@
       <c r="A58">
         <v>28</v>
       </c>
-      <c r="B58" s="14" t="s">
+      <c r="B58" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C58" s="15" t="s">
+      <c r="C58" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D58" s="15" t="s">
+      <c r="D58" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="E58" s="15" t="s">
+      <c r="E58" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="F58" s="15" t="s">
+      <c r="F58" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="G58" s="15" t="s">
+      <c r="G58" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="H58" s="15" t="s">
+      <c r="H58" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="I58" s="15" t="s">
+      <c r="I58" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="J58" s="15" t="s">
+      <c r="J58" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="K58" s="16" t="s">
+      <c r="K58" s="14" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+      <c r="A61" s="17" t="s">
         <v>48</v>
       </c>
       <c r="B61" t="s">
@@ -2384,7 +2385,8 @@
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B65" t="s">
+      <c r="A65" s="18"/>
+      <c r="B65" s="18" t="s">
         <v>42</v>
       </c>
       <c r="C65" t="s">
@@ -2392,7 +2394,7 @@
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+      <c r="A66" s="17" t="s">
         <v>50</v>
       </c>
       <c r="B66" t="s">
@@ -2415,12 +2417,13 @@
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B70" t="s">
+      <c r="A70" s="18"/>
+      <c r="B70" s="18" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+      <c r="A71" s="17" t="s">
         <v>51</v>
       </c>
       <c r="B71" t="s">
@@ -2460,8 +2463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E76D58D-6792-C449-A56A-8191A88DF2ED}">
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61:B65"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2470,236 +2473,236 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>0.91114535182331702</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>0.73684210526315697</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>0.59786476868327398</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>0.66011787819253398</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>0.903954802259887</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>0.79185520361990902</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>0.55379746835443</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>0.651769087523277</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>0.91474062660503297</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>0.75454545454545396</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>0.597122302158273</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>0.66666666666666596</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>0.90498202362609104</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>0.78341013824884798</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>0.55194805194805197</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>0.64761904761904698</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>0.90703646635849999</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>0.76576576576576505</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>0.56856187290969895</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>0.65259117082533502</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>0.89671120246659797</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>0.76954732510288004</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>0.563253012048192</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>0.65043478260869503</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>0.89362795477903301</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>0.71428571428571397</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>0.539215686274509</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>0.61452513966480404</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>0.89568345323741005</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>0.78026905829596405</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <v>0.53048780487804803</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>0.63157894736842102</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <v>0.89876670092497402</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>0.72566371681415898</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <v>0.54849498327759105</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <v>0.62476190476190396</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="6">
         <v>0.91161356628982504</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="6">
         <v>0.79757085020242902</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="6">
         <v>0.61755485893416895</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="6">
         <v>0.69611307420494695</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <f>AVERAGE(B3:B12)</f>
         <v>0.90382621483706682</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <f>AVERAGE(C3:C12)</f>
         <v>0.7619755332144279</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="5">
         <f>AVERAGE(D3:D12)</f>
         <v>0.56683008094662368</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <f>AVERAGE(E3:E12)</f>
         <v>0.64961776994356302</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
@@ -3542,31 +3545,31 @@
       <c r="A54">
         <v>24</v>
       </c>
-      <c r="B54" s="9" t="s">
+      <c r="B54" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C54" s="10" t="s">
+      <c r="C54" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D54" s="10" t="s">
+      <c r="D54" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E54" s="10" t="s">
+      <c r="E54" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="F54" s="10" t="s">
+      <c r="F54" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="G54" s="10" t="s">
+      <c r="G54" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="H54" s="10" t="s">
+      <c r="H54" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="I54" s="10" t="s">
+      <c r="I54" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="J54" s="11" t="s">
+      <c r="J54" s="9" t="s">
         <v>38</v>
       </c>
       <c r="K54" t="s">
@@ -3577,31 +3580,31 @@
       <c r="A55">
         <v>25</v>
       </c>
-      <c r="B55" s="12" t="s">
+      <c r="B55" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C55" s="8" t="s">
+      <c r="C55" t="s">
         <v>33</v>
       </c>
-      <c r="D55" s="8" t="s">
+      <c r="D55" t="s">
         <v>37</v>
       </c>
-      <c r="E55" s="8" t="s">
+      <c r="E55" t="s">
         <v>33</v>
       </c>
-      <c r="F55" s="8" t="s">
+      <c r="F55" t="s">
         <v>36</v>
       </c>
-      <c r="G55" s="8" t="s">
+      <c r="G55" t="s">
         <v>41</v>
       </c>
-      <c r="H55" s="8" t="s">
+      <c r="H55" t="s">
         <v>37</v>
       </c>
-      <c r="I55" s="8" t="s">
+      <c r="I55" t="s">
         <v>36</v>
       </c>
-      <c r="J55" s="13" t="s">
+      <c r="J55" s="11" t="s">
         <v>33</v>
       </c>
       <c r="K55" t="s">
@@ -3612,31 +3615,31 @@
       <c r="A56">
         <v>26</v>
       </c>
-      <c r="B56" s="12" t="s">
+      <c r="B56" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C56" s="8" t="s">
+      <c r="C56" t="s">
         <v>43</v>
       </c>
-      <c r="D56" s="8" t="s">
+      <c r="D56" t="s">
         <v>39</v>
       </c>
-      <c r="E56" s="8" t="s">
+      <c r="E56" t="s">
         <v>39</v>
       </c>
-      <c r="F56" s="8" t="s">
+      <c r="F56" t="s">
         <v>39</v>
       </c>
-      <c r="G56" s="8" t="s">
+      <c r="G56" t="s">
         <v>39</v>
       </c>
-      <c r="H56" s="8" t="s">
+      <c r="H56" t="s">
         <v>43</v>
       </c>
-      <c r="I56" s="8" t="s">
+      <c r="I56" t="s">
         <v>41</v>
       </c>
-      <c r="J56" s="13" t="s">
+      <c r="J56" s="11" t="s">
         <v>41</v>
       </c>
       <c r="K56" t="s">
@@ -3647,31 +3650,31 @@
       <c r="A57">
         <v>27</v>
       </c>
-      <c r="B57" s="12" t="s">
+      <c r="B57" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C57" s="8" t="s">
+      <c r="C57" t="s">
         <v>39</v>
       </c>
-      <c r="D57" s="8" t="s">
+      <c r="D57" t="s">
         <v>43</v>
       </c>
-      <c r="E57" s="8" t="s">
+      <c r="E57" t="s">
         <v>43</v>
       </c>
-      <c r="F57" s="8" t="s">
+      <c r="F57" t="s">
         <v>41</v>
       </c>
-      <c r="G57" s="8" t="s">
+      <c r="G57" t="s">
         <v>43</v>
       </c>
-      <c r="H57" s="8" t="s">
+      <c r="H57" t="s">
         <v>39</v>
       </c>
-      <c r="I57" s="8" t="s">
+      <c r="I57" t="s">
         <v>43</v>
       </c>
-      <c r="J57" s="13" t="s">
+      <c r="J57" s="11" t="s">
         <v>39</v>
       </c>
       <c r="K57" t="s">
@@ -3682,31 +3685,31 @@
       <c r="A58">
         <v>28</v>
       </c>
-      <c r="B58" s="14" t="s">
+      <c r="B58" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C58" s="15" t="s">
+      <c r="C58" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D58" s="15" t="s">
+      <c r="D58" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E58" s="15" t="s">
+      <c r="E58" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F58" s="15" t="s">
+      <c r="F58" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="G58" s="15" t="s">
+      <c r="G58" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="H58" s="15" t="s">
+      <c r="H58" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="I58" s="15" t="s">
+      <c r="I58" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="J58" s="16" t="s">
+      <c r="J58" s="14" t="s">
         <v>44</v>
       </c>
       <c r="K58" t="s">
@@ -3723,8 +3726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B09AD0DC-F606-6E4B-84BA-99ECC0FFCD33}">
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62:B66"/>
+    <sheetView topLeftCell="A6" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3733,236 +3736,236 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>0.91307773109243695</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>0.77307692307692299</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>0.65365853658536499</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>0.70837004405286297</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>0.91885504201680601</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>0.79925650557620798</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>0.68145800316957195</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>0.73567151411462794</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>0.90966386554621803</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>0.80388349514563096</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>0.63013698630136905</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>0.706484641638225</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>0.91334033613445298</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>0.77079482439925995</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>0.66934189406099498</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>0.71649484536082397</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>0.92542016806722605</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>0.78571428571428503</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>0.67266187050359705</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>0.724806201550387</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>0.91517857142857095</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>0.79411764705882304</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>0.65008025682182902</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>0.71491615180935497</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>0.92043067226890696</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>0.78723404255319096</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>0.64572425828970303</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>0.70949185043144702</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>0.91097689075630195</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>0.79473684210526296</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <v>0.67111111111111099</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>0.72771084337349301</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <v>0.91517857142857095</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>0.79411764705882304</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <v>0.65008025682182902</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <v>0.71491615180935497</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="6">
         <v>0.91832983193277296</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="6">
         <v>0.80303030303030298</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="6">
         <v>0.67194928684627497</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="6">
         <v>0.73166522864538397</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <f>AVERAGE(B3:B12)</f>
         <v>0.91604516806722636</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <f>AVERAGE(C3:C12)</f>
         <v>0.79059625157187097</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="5">
         <f>AVERAGE(D3:D12)</f>
         <v>0.65962024605116454</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <f>AVERAGE(E3:E12)</f>
         <v>0.71905274727859603</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
@@ -4805,34 +4808,34 @@
       <c r="A54">
         <v>24</v>
       </c>
-      <c r="B54" s="9" t="s">
+      <c r="B54" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C54" s="10" t="s">
+      <c r="C54" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D54" s="10" t="s">
+      <c r="D54" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="E54" s="10" t="s">
+      <c r="E54" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F54" s="10" t="s">
+      <c r="F54" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="G54" s="10" t="s">
+      <c r="G54" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="H54" s="10" t="s">
+      <c r="H54" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="I54" s="10" t="s">
+      <c r="I54" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="J54" s="10" t="s">
+      <c r="J54" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="K54" s="11" t="s">
+      <c r="K54" s="9" t="s">
         <v>31</v>
       </c>
     </row>
@@ -4840,34 +4843,34 @@
       <c r="A55">
         <v>25</v>
       </c>
-      <c r="B55" s="12" t="s">
+      <c r="B55" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C55" s="8" t="s">
+      <c r="C55" t="s">
         <v>39</v>
       </c>
-      <c r="D55" s="8" t="s">
+      <c r="D55" t="s">
         <v>39</v>
       </c>
-      <c r="E55" s="8" t="s">
+      <c r="E55" t="s">
         <v>42</v>
       </c>
-      <c r="F55" s="8" t="s">
+      <c r="F55" t="s">
         <v>46</v>
       </c>
-      <c r="G55" s="8" t="s">
+      <c r="G55" t="s">
         <v>43</v>
       </c>
-      <c r="H55" s="8" t="s">
+      <c r="H55" t="s">
         <v>39</v>
       </c>
-      <c r="I55" s="8" t="s">
+      <c r="I55" t="s">
         <v>42</v>
       </c>
-      <c r="J55" s="8" t="s">
+      <c r="J55" t="s">
         <v>46</v>
       </c>
-      <c r="K55" s="13" t="s">
+      <c r="K55" s="11" t="s">
         <v>46</v>
       </c>
     </row>
@@ -4875,34 +4878,34 @@
       <c r="A56">
         <v>26</v>
       </c>
-      <c r="B56" s="12" t="s">
+      <c r="B56" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C56" s="8" t="s">
+      <c r="C56" t="s">
         <v>42</v>
       </c>
-      <c r="D56" s="8" t="s">
+      <c r="D56" t="s">
         <v>42</v>
       </c>
-      <c r="E56" s="8" t="s">
+      <c r="E56" t="s">
         <v>39</v>
       </c>
-      <c r="F56" s="8" t="s">
+      <c r="F56" t="s">
         <v>42</v>
       </c>
-      <c r="G56" s="8" t="s">
+      <c r="G56" t="s">
         <v>39</v>
       </c>
-      <c r="H56" s="8" t="s">
+      <c r="H56" t="s">
         <v>43</v>
       </c>
-      <c r="I56" s="8" t="s">
+      <c r="I56" t="s">
         <v>39</v>
       </c>
-      <c r="J56" s="8" t="s">
+      <c r="J56" t="s">
         <v>39</v>
       </c>
-      <c r="K56" s="13" t="s">
+      <c r="K56" s="11" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4910,34 +4913,34 @@
       <c r="A57">
         <v>27</v>
       </c>
-      <c r="B57" s="12" t="s">
+      <c r="B57" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C57" s="8" t="s">
+      <c r="C57" t="s">
         <v>45</v>
       </c>
-      <c r="D57" s="8" t="s">
+      <c r="D57" t="s">
         <v>45</v>
       </c>
-      <c r="E57" s="8" t="s">
+      <c r="E57" t="s">
         <v>45</v>
       </c>
-      <c r="F57" s="8" t="s">
+      <c r="F57" t="s">
         <v>45</v>
       </c>
-      <c r="G57" s="8" t="s">
+      <c r="G57" t="s">
         <v>45</v>
       </c>
-      <c r="H57" s="8" t="s">
+      <c r="H57" t="s">
         <v>45</v>
       </c>
-      <c r="I57" s="8" t="s">
+      <c r="I57" t="s">
         <v>45</v>
       </c>
-      <c r="J57" s="8" t="s">
+      <c r="J57" t="s">
         <v>45</v>
       </c>
-      <c r="K57" s="13" t="s">
+      <c r="K57" s="11" t="s">
         <v>45</v>
       </c>
     </row>
@@ -4945,34 +4948,34 @@
       <c r="A58">
         <v>28</v>
       </c>
-      <c r="B58" s="14" t="s">
+      <c r="B58" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C58" s="15" t="s">
+      <c r="C58" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D58" s="15" t="s">
+      <c r="D58" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E58" s="15" t="s">
+      <c r="E58" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F58" s="15" t="s">
+      <c r="F58" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="G58" s="15" t="s">
+      <c r="G58" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="H58" s="15" t="s">
+      <c r="H58" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="I58" s="15" t="s">
+      <c r="I58" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="J58" s="15" t="s">
+      <c r="J58" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="K58" s="16" t="s">
+      <c r="K58" s="14" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>